<commit_message>
i have added call ctest class and extend report and log 4j
</commit_message>
<xml_diff>
--- a/src/main/java/crm/testData/CRM pro.xlsx
+++ b/src/main/java/crm/testData/CRM pro.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21810" windowHeight="12045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="calldata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:V38"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>title</t>
   </si>
@@ -73,6 +75,48 @@
   </si>
   <si>
     <t>rrr</t>
+  </si>
+  <si>
+    <t>deal</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
 </sst>
 </file>
@@ -403,7 +447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -488,4 +532,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>